<commit_message>
link description sfp lw
</commit_message>
<xml_diff>
--- a/dtln_device_location.xlsx
+++ b/dtln_device_location.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20394"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20395"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kavlasenko\Documents\05.PYTHON\Projects\san_report_automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E050826D-C007-4FBC-818E-414D5EA6D820}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DD2C4581-7046-4DB5-B337-B1F938C5F48B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="34335" windowHeight="11730" xr2:uid="{224B2F82-8F05-438B-BF5A-3CD3FE39A21B}"/>
   </bookViews>
   <sheets>
     <sheet name="switch_rack" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191029" iterateDelta="1E-4"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="106">
   <si>
     <t>san01-nord</t>
   </si>
@@ -325,6 +325,24 @@
   </si>
   <si>
     <t>Device_Rack</t>
+  </si>
+  <si>
+    <t>n1-g620-005-vc67-f1</t>
+  </si>
+  <si>
+    <t>n1-g620-006-vc67-f2</t>
+  </si>
+  <si>
+    <t>3H1J110 un37</t>
+  </si>
+  <si>
+    <t>3H1J090 un37</t>
+  </si>
+  <si>
+    <t>10:00:88:94:71:60:75:63</t>
+  </si>
+  <si>
+    <t>10:00:88:94:71:ce:bf:fa</t>
   </si>
 </sst>
 </file>
@@ -708,10 +726,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FE7DAD2-DE8B-4AD9-A367-2ED64EC8ED26}">
-  <dimension ref="A1:E30"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -946,36 +964,36 @@
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="C14" s="3" t="s">
-        <v>31</v>
+        <v>100</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>104</v>
       </c>
       <c r="D14" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="E14" s="3" t="s">
-        <v>83</v>
+      <c r="E14" s="1" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>13</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>32</v>
+        <v>101</v>
+      </c>
+      <c r="C15" s="1" t="s">
+        <v>105</v>
       </c>
       <c r="D15" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>81</v>
+        <v>36</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>103</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.25">
@@ -983,16 +1001,16 @@
         <v>17</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>36</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.25">
@@ -1000,84 +1018,84 @@
         <v>17</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>37</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>42</v>
+        <v>17</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>14</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>55</v>
+        <v>33</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>36</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B19" s="3" t="s">
-        <v>43</v>
+        <v>17</v>
+      </c>
+      <c r="B19" s="1" t="s">
+        <v>15</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>56</v>
+        <v>34</v>
       </c>
       <c r="D19" s="3" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B20" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="D20" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="D21" s="3" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E21" s="3" t="s">
-        <v>89</v>
+        <v>86</v>
       </c>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.25">
@@ -1085,16 +1103,16 @@
         <v>40</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>37</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.25">
@@ -1102,16 +1120,16 @@
         <v>40</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C23" s="3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D23" s="3" t="s">
         <v>37</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>88</v>
+        <v>89</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
@@ -1119,16 +1137,16 @@
         <v>40</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C24" s="3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D24" s="3" t="s">
         <v>37</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.25">
@@ -1136,16 +1154,16 @@
         <v>40</v>
       </c>
       <c r="B25" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C25" s="3" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>37</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.25">
@@ -1153,47 +1171,47 @@
         <v>40</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C26" s="3" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="D26" s="3" t="s">
-        <v>68</v>
+        <v>37</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>90</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B27" s="3" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C27" s="3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="D27" s="3" t="s">
         <v>37</v>
       </c>
       <c r="E27" s="3" t="s">
-        <v>95</v>
+        <v>92</v>
       </c>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B28" s="3" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E28" s="3" t="s">
-        <v>93</v>
+        <v>68</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
@@ -1201,16 +1219,16 @@
         <v>41</v>
       </c>
       <c r="B29" s="3" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C29" s="3" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="D29" s="3" t="s">
         <v>37</v>
       </c>
       <c r="E29" s="3" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.25">
@@ -1218,15 +1236,49 @@
         <v>41</v>
       </c>
       <c r="B30" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C30" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="D30" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E30" s="3" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C31" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D31" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B32" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="C30" s="3" t="s">
+      <c r="C32" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="D30" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="E30" s="3" t="s">
+      <c r="D32" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="E32" s="3" t="s">
         <v>94</v>
       </c>
     </row>

</xml_diff>

<commit_message>
port statistics device class npiv tag
</commit_message>
<xml_diff>
--- a/dtln_device_location.xlsx
+++ b/dtln_device_location.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kavlasenko\Documents\05.PYTHON\Projects\san_report_automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0683801C-576F-4DA4-8F2E-D7DA56CF1FD0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EF86694-4388-477C-8070-C7FC78C3AC8F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="34335" windowHeight="11730" xr2:uid="{224B2F82-8F05-438B-BF5A-3CD3FE39A21B}"/>
+    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="34335" windowHeight="11730" xr2:uid="{224B2F82-8F05-438B-BF5A-3CD3FE39A21B}"/>
   </bookViews>
   <sheets>
     <sheet name="switch_rack" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="188">
   <si>
     <t>san01-nord</t>
   </si>
@@ -402,9 +402,6 @@
     <t>10:00:50:eb:1a:84:7d:95</t>
   </si>
   <si>
-    <t>Brocade 300 Switch</t>
-  </si>
-  <si>
     <t>san67-ost</t>
   </si>
   <si>
@@ -481,6 +478,117 @@
   </si>
   <si>
     <t>SPVB</t>
+  </si>
+  <si>
+    <t>san61-nord</t>
+  </si>
+  <si>
+    <t>san62-nord</t>
+  </si>
+  <si>
+    <t>10:00:d8:1f:cc:01:23:c0</t>
+  </si>
+  <si>
+    <t>10:00:d8:1f:cc:01:24:80</t>
+  </si>
+  <si>
+    <t>Brocade G610</t>
+  </si>
+  <si>
+    <t>6H4E020 un39</t>
+  </si>
+  <si>
+    <t>6H4E010 un39</t>
+  </si>
+  <si>
+    <t>Ruexce</t>
+  </si>
+  <si>
+    <t>Cit</t>
+  </si>
+  <si>
+    <t>nsk-6505-73-f1-cit</t>
+  </si>
+  <si>
+    <t>nsk-6505-74-f2-cit</t>
+  </si>
+  <si>
+    <t>10:00:88:94:71:71:95:ac</t>
+  </si>
+  <si>
+    <t>10:00:88:94:71:71:9b:24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NSK_2_4_14 un23	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">NSK_2_4_14 un25	</t>
+  </si>
+  <si>
+    <t>Hoff</t>
+  </si>
+  <si>
+    <t>san63-nord</t>
+  </si>
+  <si>
+    <t>san64-nord</t>
+  </si>
+  <si>
+    <t>Brocade 300</t>
+  </si>
+  <si>
+    <t>3H1L080 u37</t>
+  </si>
+  <si>
+    <t>3H1L080 u35</t>
+  </si>
+  <si>
+    <t>10:00:88:94:71:3d:68:80</t>
+  </si>
+  <si>
+    <t>10:00:88:94:71:3d:66:20</t>
+  </si>
+  <si>
+    <t>Efes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">san113-nord	</t>
+  </si>
+  <si>
+    <t xml:space="preserve">san114-nord	</t>
+  </si>
+  <si>
+    <t>3H1J030 un41</t>
+  </si>
+  <si>
+    <t>3H1J010 un41</t>
+  </si>
+  <si>
+    <t>10:00:00:27:f8:0b:f4:81</t>
+  </si>
+  <si>
+    <t>10:00:00:27:f8:0a:ff:e6</t>
+  </si>
+  <si>
+    <t>OST STG</t>
+  </si>
+  <si>
+    <t>o2-6505-05-stg-f1</t>
+  </si>
+  <si>
+    <t>o2-6505-06-stg-f2</t>
+  </si>
+  <si>
+    <t>1H10A040 un42</t>
+  </si>
+  <si>
+    <t>1H10A040 un41</t>
+  </si>
+  <si>
+    <t>10:00:c4:f5:7c:8f:29:38</t>
+  </si>
+  <si>
+    <t>10:00:c4:f5:7c:8f:43:98</t>
   </si>
 </sst>
 </file>
@@ -864,10 +972,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FE7DAD2-DE8B-4AD9-A367-2ED64EC8ED26}">
-  <dimension ref="A1:E45"/>
+  <dimension ref="A1:E55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="F33" sqref="F32:F33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1513,16 +1621,16 @@
         <v>116</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C38" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="D38" s="3" t="s">
-        <v>125</v>
+      <c r="D38" s="1" t="s">
+        <v>169</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
@@ -1530,118 +1638,288 @@
         <v>116</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="D39" s="3" t="s">
-        <v>125</v>
+        <v>128</v>
+      </c>
+      <c r="D39" s="1" t="s">
+        <v>169</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="B40" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="B40" s="1" t="s">
-        <v>132</v>
-      </c>
       <c r="C40" s="1" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>36</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B41" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>36</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="1" t="s">
+      <c r="A42" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="B42" s="1" t="s">
         <v>138</v>
       </c>
-      <c r="B42" s="1" t="s">
-        <v>139</v>
-      </c>
       <c r="C42" s="1" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>36</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="1" t="s">
-        <v>138</v>
+      <c r="A43" s="3" t="s">
+        <v>137</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>36</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="1" t="s">
-        <v>151</v>
+      <c r="A44" s="3" t="s">
+        <v>150</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>36</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="1" t="s">
-        <v>151</v>
+      <c r="A45" s="3" t="s">
+        <v>150</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>36</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="E47" s="1" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A48" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="C48" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="D48" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E48" s="1" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A49" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="C49" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="D49" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E49" s="1" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A50" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>167</v>
+      </c>
+      <c r="C50" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="D50" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E50" s="1" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A51" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="C51" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="D51" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E51" s="1" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A52" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="E52" s="1" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A53" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="E53" s="1" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A54" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B54" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E54" s="1" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A55" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B55" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="C55" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E55" s="1" t="s">
+        <v>185</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
freezed domain names functionality
</commit_message>
<xml_diff>
--- a/dtln_device_location.xlsx
+++ b/dtln_device_location.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kavlasenko\Documents\05.PYTHON\Projects\san_report_automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EF86694-4388-477C-8070-C7FC78C3AC8F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33AC7FF3-16F5-4950-B4AF-4F0069ED2ABA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="0" yWindow="0" windowWidth="34335" windowHeight="11730" xr2:uid="{224B2F82-8F05-438B-BF5A-3CD3FE39A21B}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="34335" windowHeight="11730" xr2:uid="{224B2F82-8F05-438B-BF5A-3CD3FE39A21B}"/>
   </bookViews>
   <sheets>
     <sheet name="switch_rack" sheetId="1" r:id="rId1"/>
+    <sheet name="Лист1" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="275" uniqueCount="188">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="231">
   <si>
     <t>san01-nord</t>
   </si>
@@ -447,12 +448,6 @@
     <t>san46-udm</t>
   </si>
   <si>
-    <t>UDM 4_12_13 un35</t>
-  </si>
-  <si>
-    <t>UDM 4_12_15 un35</t>
-  </si>
-  <si>
     <t>10:00:d8:1f:cc:06:26:7a</t>
   </si>
   <si>
@@ -465,12 +460,6 @@
     <t xml:space="preserve">san112-spb	</t>
   </si>
   <si>
-    <t>SPB 3_2_10 un37</t>
-  </si>
-  <si>
-    <t>SPB 3_2_11 un37</t>
-  </si>
-  <si>
     <t>10:00:d8:1f:cc:7c:cb:e0</t>
   </si>
   <si>
@@ -589,13 +578,154 @@
   </si>
   <si>
     <t>10:00:c4:f5:7c:8f:43:98</t>
+  </si>
+  <si>
+    <t>san77-nord</t>
+  </si>
+  <si>
+    <t>san79-nord</t>
+  </si>
+  <si>
+    <t>san81-nord</t>
+  </si>
+  <si>
+    <t>san78-nord</t>
+  </si>
+  <si>
+    <t>san80-nord</t>
+  </si>
+  <si>
+    <t>san82-nord</t>
+  </si>
+  <si>
+    <t>san83-ost</t>
+  </si>
+  <si>
+    <t>san85-ost</t>
+  </si>
+  <si>
+    <t>san87-ost</t>
+  </si>
+  <si>
+    <t>san89-ost</t>
+  </si>
+  <si>
+    <t>san84-ost</t>
+  </si>
+  <si>
+    <t>san86-ost</t>
+  </si>
+  <si>
+    <t>san88-ost</t>
+  </si>
+  <si>
+    <t>san90-ost</t>
+  </si>
+  <si>
+    <t>10:00:50:eb:1a:2a:fc:9b</t>
+  </si>
+  <si>
+    <t>10:00:50:eb:1a:2a:84:b5</t>
+  </si>
+  <si>
+    <t>10:00:c4:f5:7c:80:bd:08</t>
+  </si>
+  <si>
+    <t>10:00:50:eb:1a:2a:df:57</t>
+  </si>
+  <si>
+    <t>10:00:50:eb:1a:2a:de:67</t>
+  </si>
+  <si>
+    <t>10:00:c4:f5:7c:80:ad:d0</t>
+  </si>
+  <si>
+    <t>10:00:00:05:33:ac:74:ed</t>
+  </si>
+  <si>
+    <t>10:00:00:27:f8:d1:22:34</t>
+  </si>
+  <si>
+    <t>10:00:c4:f5:7c:22:ce:28</t>
+  </si>
+  <si>
+    <t>10:00:c4:f5:7c:21:7e:2c</t>
+  </si>
+  <si>
+    <t>10:00:00:05:33:ad:25:ff</t>
+  </si>
+  <si>
+    <t>10:00:00:27:f8:d1:22:94</t>
+  </si>
+  <si>
+    <t>10:00:c4:f5:7c:21:9f:4d</t>
+  </si>
+  <si>
+    <t>10:00:c4:f5:7c:21:a0:0d</t>
+  </si>
+  <si>
+    <t>Kaspersky</t>
+  </si>
+  <si>
+    <t>4H3J005 un37</t>
+  </si>
+  <si>
+    <t>4H3J010 un34</t>
+  </si>
+  <si>
+    <t>4H2H070 un34</t>
+  </si>
+  <si>
+    <t>4H2H080 un34</t>
+  </si>
+  <si>
+    <t>4H2H090 un26</t>
+  </si>
+  <si>
+    <t>4H2H090 un30</t>
+  </si>
+  <si>
+    <t>H6G160 u42</t>
+  </si>
+  <si>
+    <t>H6G160 u41</t>
+  </si>
+  <si>
+    <t>H10B030 u36</t>
+  </si>
+  <si>
+    <t>H10B030 u34</t>
+  </si>
+  <si>
+    <t>H3D085 u35</t>
+  </si>
+  <si>
+    <t>H3D090 u35</t>
+  </si>
+  <si>
+    <t>H3D085 u32</t>
+  </si>
+  <si>
+    <t>H3D090 u32</t>
+  </si>
+  <si>
+    <t>UDM_4_12_13 un35</t>
+  </si>
+  <si>
+    <t>UDM_4_12_15 un35</t>
+  </si>
+  <si>
+    <t>SPB_3_2_11 un37</t>
+  </si>
+  <si>
+    <t>SPB_3_2_10 un37</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -625,6 +755,10 @@
       <family val="2"/>
       <charset val="204"/>
     </font>
+    <font>
+      <sz val="10"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -652,12 +786,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
@@ -972,10 +1107,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FE7DAD2-DE8B-4AD9-A367-2ED64EC8ED26}">
-  <dimension ref="A1:E55"/>
+  <dimension ref="A1:E69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="F33" sqref="F32:F33"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="E49" sqref="E49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1627,7 +1762,7 @@
         <v>124</v>
       </c>
       <c r="D38" s="1" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="E38" s="1" t="s">
         <v>126</v>
@@ -1644,7 +1779,7 @@
         <v>128</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="E39" s="1" t="s">
         <v>127</v>
@@ -1692,13 +1827,13 @@
         <v>138</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>36</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>140</v>
+        <v>227</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
@@ -1709,217 +1844,587 @@
         <v>139</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>36</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>141</v>
+        <v>228</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B44" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="C44" s="1" t="s">
         <v>144</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>148</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>36</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>147</v>
+        <v>229</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="B45" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="C45" s="1" t="s">
         <v>145</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>149</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>36</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>146</v>
+        <v>230</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B46" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="D46" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="C46" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>155</v>
-      </c>
       <c r="E46" s="1" t="s">
-        <v>156</v>
+        <v>152</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>152</v>
+        <v>148</v>
       </c>
       <c r="C47" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="E47" s="1" t="s">
         <v>153</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="E47" s="1" t="s">
-        <v>157</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>159</v>
+        <v>155</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>162</v>
+        <v>158</v>
       </c>
       <c r="D48" s="1" t="s">
         <v>120</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>164</v>
+        <v>160</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
+        <v>155</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="C49" s="1" t="s">
         <v>159</v>
-      </c>
-      <c r="B49" s="1" t="s">
-        <v>161</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>163</v>
       </c>
       <c r="D49" s="1" t="s">
         <v>120</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>165</v>
+        <v>161</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>167</v>
+        <v>163</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>120</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>166</v>
+        <v>162</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>168</v>
+        <v>164</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>120</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>174</v>
+        <v>170</v>
       </c>
       <c r="B52" s="1" t="s">
+        <v>171</v>
+      </c>
+      <c r="C52" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="C52" s="1" t="s">
-        <v>179</v>
-      </c>
       <c r="D52" s="1" t="s">
-        <v>169</v>
+        <v>165</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="C53" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="E53" s="1" t="s">
         <v>174</v>
-      </c>
-      <c r="B53" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>180</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>169</v>
-      </c>
-      <c r="E53" s="1" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="B54" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="C54" s="1" t="s">
         <v>182</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>186</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>120</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="B55" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="C55" s="1" t="s">
         <v>183</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>187</v>
       </c>
       <c r="D55" s="1" t="s">
         <v>120</v>
       </c>
       <c r="E55" s="1" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A56" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="B56" s="5" t="s">
+        <v>184</v>
+      </c>
+      <c r="C56" s="5" t="s">
+        <v>198</v>
+      </c>
+      <c r="D56" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="E56" s="1" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A57" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="B57" s="5" t="s">
         <v>185</v>
+      </c>
+      <c r="C57" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="D57" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="E57" s="1" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A58" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="B58" s="5" t="s">
+        <v>186</v>
+      </c>
+      <c r="C58" s="5" t="s">
+        <v>200</v>
+      </c>
+      <c r="D58" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="E58" s="1" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A59" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="B59" s="5" t="s">
+        <v>187</v>
+      </c>
+      <c r="C59" s="5" t="s">
+        <v>201</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="E59" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A60" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="B60" s="5" t="s">
+        <v>188</v>
+      </c>
+      <c r="C60" s="5" t="s">
+        <v>202</v>
+      </c>
+      <c r="D60" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="E60" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A61" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="B61" s="5" t="s">
+        <v>189</v>
+      </c>
+      <c r="C61" s="5" t="s">
+        <v>203</v>
+      </c>
+      <c r="D61" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="E61" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A62" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="B62" s="5" t="s">
+        <v>190</v>
+      </c>
+      <c r="C62" s="5" t="s">
+        <v>204</v>
+      </c>
+      <c r="D62" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="E62" s="1" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A63" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="B63" s="5" t="s">
+        <v>191</v>
+      </c>
+      <c r="C63" s="5" t="s">
+        <v>205</v>
+      </c>
+      <c r="D63" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="E63" s="1" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A64" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="B64" s="5" t="s">
+        <v>192</v>
+      </c>
+      <c r="C64" s="5" t="s">
+        <v>206</v>
+      </c>
+      <c r="D64" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="E64" s="1" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A65" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="B65" s="5" t="s">
+        <v>193</v>
+      </c>
+      <c r="C65" s="5" t="s">
+        <v>207</v>
+      </c>
+      <c r="D65" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="E65" s="1" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A66" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="B66" s="5" t="s">
+        <v>194</v>
+      </c>
+      <c r="C66" s="5" t="s">
+        <v>208</v>
+      </c>
+      <c r="D66" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="E66" s="1" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A67" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="B67" s="5" t="s">
+        <v>195</v>
+      </c>
+      <c r="C67" s="5" t="s">
+        <v>209</v>
+      </c>
+      <c r="D67" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="E67" s="1" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A68" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="B68" s="5" t="s">
+        <v>196</v>
+      </c>
+      <c r="C68" s="5" t="s">
+        <v>210</v>
+      </c>
+      <c r="D68" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="E68" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A69" s="1" t="s">
+        <v>212</v>
+      </c>
+      <c r="B69" s="5" t="s">
+        <v>197</v>
+      </c>
+      <c r="C69" s="5" t="s">
+        <v>211</v>
+      </c>
+      <c r="D69" s="1" t="s">
+        <v>165</v>
+      </c>
+      <c r="E69" s="1" t="s">
+        <v>226</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8715A167-603C-4A29-BCE5-E60E3FF0DC4C}">
+  <dimension ref="A1:B14"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.140625" customWidth="1"/>
+    <col min="2" max="2" width="29.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>184</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>185</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" s="1" t="s">
+        <v>194</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" s="1" t="s">
+        <v>195</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>222</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" s="1" t="s">
+        <v>192</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" s="1" t="s">
+        <v>196</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" s="1" t="s">
+        <v>193</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" s="1" t="s">
+        <v>197</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>226</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
raslog severe latency description added
</commit_message>
<xml_diff>
--- a/dtln_device_location.xlsx
+++ b/dtln_device_location.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kavlasenko\Documents\05.PYTHON\Projects\san_report_automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33AC7FF3-16F5-4950-B4AF-4F0069ED2ABA}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{486F8F1B-3D33-4B48-8B49-3747FDA6D1F9}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="34335" windowHeight="11730" xr2:uid="{224B2F82-8F05-438B-BF5A-3CD3FE39A21B}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="403" uniqueCount="251">
   <si>
     <t>san01-nord</t>
   </si>
@@ -343,18 +343,12 @@
     <t>10:00:88:94:71:ee:37:e0</t>
   </si>
   <si>
-    <t>6H1L090</t>
-  </si>
-  <si>
     <t>san69-nord</t>
   </si>
   <si>
     <t>10:00:88:94:71:2e:c3:c4</t>
   </si>
   <si>
-    <t>6H1L100</t>
-  </si>
-  <si>
     <t>san70-nord</t>
   </si>
   <si>
@@ -719,6 +713,72 @@
   </si>
   <si>
     <t>SPB_3_2_10 un37</t>
+  </si>
+  <si>
+    <t>6H1L090 un37</t>
+  </si>
+  <si>
+    <t>6H1L100 un37</t>
+  </si>
+  <si>
+    <t>10:00:d8:1f:cc:7c:cc:40</t>
+  </si>
+  <si>
+    <t>10:00:d8:1f:cc:7c:c8:e0</t>
+  </si>
+  <si>
+    <t>5H1I095 un39</t>
+  </si>
+  <si>
+    <t>5H1I095 un37</t>
+  </si>
+  <si>
+    <t>NORD STG</t>
+  </si>
+  <si>
+    <t>n3-g620-117-stg-f1</t>
+  </si>
+  <si>
+    <t>n3-g620-118-stg-f2</t>
+  </si>
+  <si>
+    <t>10:00:00:27:f8:0c:65:42</t>
+  </si>
+  <si>
+    <t>san41-ost</t>
+  </si>
+  <si>
+    <t>10:00:00:27:f8:0c:7c:82</t>
+  </si>
+  <si>
+    <t>san42-ost</t>
+  </si>
+  <si>
+    <t>10:00:00:27:f8:bd:34:18</t>
+  </si>
+  <si>
+    <t>10:00:00:27:f8:bd:48:58</t>
+  </si>
+  <si>
+    <t>san39-nord</t>
+  </si>
+  <si>
+    <t>san40-nord</t>
+  </si>
+  <si>
+    <t>Internal</t>
+  </si>
+  <si>
+    <t>5H3C060 un37</t>
+  </si>
+  <si>
+    <t>5H3C060 un38</t>
+  </si>
+  <si>
+    <t>H6E020 un39</t>
+  </si>
+  <si>
+    <t>H6E020 un40</t>
   </si>
 </sst>
 </file>
@@ -758,6 +818,8 @@
     <font>
       <sz val="10"/>
       <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
     </font>
   </fonts>
   <fills count="3">
@@ -1107,10 +1169,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FE7DAD2-DE8B-4AD9-A367-2ED64EC8ED26}">
-  <dimension ref="A1:E69"/>
+  <dimension ref="A1:E75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
-      <selection activeCell="E49" sqref="E49"/>
+    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
+      <selection activeCell="E69" sqref="E69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1651,7 +1713,7 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>103</v>
@@ -1663,636 +1725,738 @@
         <v>37</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>105</v>
+        <v>229</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B33" s="3" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C33" s="3" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="D33" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="E33" s="3" t="s">
-        <v>108</v>
+      <c r="E33" s="1" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B34" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="C34" s="3" t="s">
         <v>106</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>107</v>
       </c>
       <c r="D34" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="E34" s="3" t="s">
-        <v>111</v>
+      <c r="E34" s="1" t="s">
+        <v>109</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="C35" s="3" t="s">
         <v>113</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>115</v>
       </c>
       <c r="D35" s="3" t="s">
         <v>37</v>
       </c>
       <c r="E35" s="3" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B36" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="B36" s="3" t="s">
+      <c r="C36" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="D36" s="3" t="s">
         <v>118</v>
       </c>
-      <c r="C36" s="3" t="s">
+      <c r="E36" s="1" t="s">
         <v>117</v>
-      </c>
-      <c r="D36" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="E36" s="3" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C37" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="D37" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="E37" s="3" t="s">
         <v>121</v>
-      </c>
-      <c r="D37" s="3" t="s">
-        <v>120</v>
-      </c>
-      <c r="E37" s="3" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="C38" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="D38" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="E38" s="1" t="s">
         <v>124</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="E38" s="1" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="B39" s="1" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="D39" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E39" s="1" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C40" s="1" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="D40" s="1" t="s">
         <v>36</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B41" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="B41" s="1" t="s">
-        <v>132</v>
-      </c>
       <c r="C41" s="1" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="D41" s="1" t="s">
         <v>36</v>
       </c>
       <c r="E41" s="1" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B42" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="C42" s="1" t="s">
         <v>138</v>
-      </c>
-      <c r="C42" s="1" t="s">
-        <v>140</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>36</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="B43" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="B43" s="1" t="s">
+      <c r="C43" s="1" t="s">
         <v>139</v>
-      </c>
-      <c r="C43" s="1" t="s">
-        <v>141</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>36</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>228</v>
+        <v>226</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B44" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C44" s="1" t="s">
         <v>142</v>
-      </c>
-      <c r="C44" s="1" t="s">
-        <v>144</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>36</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>229</v>
+        <v>227</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="B45" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C45" s="1" t="s">
         <v>143</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>145</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>36</v>
       </c>
       <c r="E45" s="1" t="s">
-        <v>230</v>
+        <v>228</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="C46" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="E46" s="1" t="s">
         <v>150</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>152</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>154</v>
+        <v>152</v>
       </c>
       <c r="B47" s="1" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C47" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="D47" s="1" t="s">
         <v>149</v>
       </c>
-      <c r="D47" s="1" t="s">
+      <c r="E47" s="1" t="s">
         <v>151</v>
-      </c>
-      <c r="E47" s="1" t="s">
-        <v>153</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="B48" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="C48" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="C48" s="1" t="s">
+      <c r="D48" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="E48" s="1" t="s">
         <v>158</v>
-      </c>
-      <c r="D48" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="E48" s="1" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B49" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="B49" s="1" t="s">
+      <c r="C49" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="C49" s="1" t="s">
+      <c r="D49" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="E49" s="1" t="s">
         <v>159</v>
-      </c>
-      <c r="D49" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="E49" s="1" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D50" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B51" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="B51" s="1" t="s">
-        <v>164</v>
-      </c>
       <c r="C51" s="1" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="D51" s="1" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="B52" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="C52" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="D52" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="E52" s="1" t="s">
         <v>171</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>175</v>
-      </c>
-      <c r="D52" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="E52" s="1" t="s">
-        <v>173</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B53" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="B53" s="1" t="s">
+      <c r="C53" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="D53" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="E53" s="1" t="s">
         <v>172</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>176</v>
-      </c>
-      <c r="D53" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="E53" s="1" t="s">
-        <v>174</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>177</v>
+        <v>175</v>
       </c>
       <c r="B54" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="C54" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="D54" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="E54" s="1" t="s">
         <v>178</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>182</v>
-      </c>
-      <c r="D54" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="E54" s="1" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B55" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="B55" s="1" t="s">
+      <c r="C55" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="D55" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="E55" s="1" t="s">
         <v>179</v>
-      </c>
-      <c r="C55" s="1" t="s">
-        <v>183</v>
-      </c>
-      <c r="D55" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="E55" s="1" t="s">
-        <v>181</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B56" s="5" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C56" s="5" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B57" s="5" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C57" s="5" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D58" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
+        <v>210</v>
+      </c>
+      <c r="B59" s="5" t="s">
+        <v>185</v>
+      </c>
+      <c r="C59" s="5" t="s">
+        <v>199</v>
+      </c>
+      <c r="D59" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="E59" s="1" t="s">
         <v>212</v>
-      </c>
-      <c r="B59" s="5" t="s">
-        <v>187</v>
-      </c>
-      <c r="C59" s="5" t="s">
-        <v>201</v>
-      </c>
-      <c r="D59" s="1" t="s">
-        <v>165</v>
-      </c>
-      <c r="E59" s="1" t="s">
-        <v>214</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C60" s="5" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D60" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C61" s="5" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D61" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C62" s="5" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D62" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C63" s="5" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D63" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C64" s="5" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B65" s="5" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C65" s="5" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D65" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C66" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D66" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C67" s="5" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D67" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="C68" s="5" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
       <c r="D68" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B69" s="5" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="C69" s="5" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="D69" s="1" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>226</v>
+        <v>224</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A70" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="B70" s="5" t="s">
+        <v>236</v>
+      </c>
+      <c r="C70" s="5" t="s">
+        <v>231</v>
+      </c>
+      <c r="D70" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E70" s="1" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
+        <v>235</v>
+      </c>
+      <c r="B71" s="5" t="s">
+        <v>237</v>
+      </c>
+      <c r="C71" s="5" t="s">
+        <v>232</v>
+      </c>
+      <c r="D71" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E71" s="1" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A72" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="B72" s="5" t="s">
+        <v>244</v>
+      </c>
+      <c r="C72" s="1" t="s">
+        <v>242</v>
+      </c>
+      <c r="D72" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="E72" s="1" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A73" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="B73" s="5" t="s">
+        <v>245</v>
+      </c>
+      <c r="C73" s="1" t="s">
+        <v>243</v>
+      </c>
+      <c r="D73" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="E73" s="1" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A74" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="B74" s="5" t="s">
+        <v>239</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>238</v>
+      </c>
+      <c r="D74" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="E74" s="1" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="B75" s="5" t="s">
+        <v>241</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="D75" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="E75" s="1" t="s">
+        <v>250</v>
       </c>
     </row>
   </sheetData>
@@ -2317,114 +2481,114 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>196</v>
+        <v>194</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>197</v>
+        <v>195</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
infinidat node port name from wwn
</commit_message>
<xml_diff>
--- a/dtln_device_location.xlsx
+++ b/dtln_device_location.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20398"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20399"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kavlasenko\Documents\05.PYTHON\Projects\san_report_automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{985AC56D-399F-4811-B01F-9DE44E60ED0E}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D394E317-781C-4791-9D26-30E79C37C1AE}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="34335" windowHeight="11730" xr2:uid="{224B2F82-8F05-438B-BF5A-3CD3FE39A21B}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="453" uniqueCount="285">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="463" uniqueCount="292">
   <si>
     <t>san01-nord</t>
   </si>
@@ -881,6 +881,27 @@
   </si>
   <si>
     <t>H13F920 un46</t>
+  </si>
+  <si>
+    <t>SPb</t>
+  </si>
+  <si>
+    <t>san13-spb</t>
+  </si>
+  <si>
+    <t>san14-spb</t>
+  </si>
+  <si>
+    <t>10:00:c4:f5:7c:4e:b0:04</t>
+  </si>
+  <si>
+    <t>10:00:c4:f5:7c:4e:87:a4</t>
+  </si>
+  <si>
+    <t>51H1B130 un38</t>
+  </si>
+  <si>
+    <t>51H1B110 un38</t>
   </si>
 </sst>
 </file>
@@ -1276,10 +1297,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FE7DAD2-DE8B-4AD9-A367-2ED64EC8ED26}">
-  <dimension ref="A1:E85"/>
+  <dimension ref="A1:E87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A61" workbookViewId="0">
-      <selection activeCell="K91" sqref="K91"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1820,53 +1841,53 @@
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>111</v>
+        <v>285</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>103</v>
+        <v>286</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="D32" s="3" t="s">
-        <v>37</v>
+        <v>288</v>
+      </c>
+      <c r="D32" s="1" t="s">
+        <v>163</v>
       </c>
       <c r="E32" s="1" t="s">
-        <v>229</v>
+        <v>290</v>
       </c>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="B33" s="3" t="s">
-        <v>108</v>
-      </c>
-      <c r="C33" s="3" t="s">
-        <v>112</v>
-      </c>
-      <c r="D33" s="3" t="s">
-        <v>37</v>
+        <v>285</v>
+      </c>
+      <c r="B33" s="1" t="s">
+        <v>287</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>289</v>
+      </c>
+      <c r="D33" s="1" t="s">
+        <v>163</v>
       </c>
       <c r="E33" s="1" t="s">
-        <v>230</v>
+        <v>291</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="B34" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="C34" s="3" t="s">
-        <v>106</v>
+      <c r="B34" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C34" s="1" t="s">
+        <v>104</v>
       </c>
       <c r="D34" s="3" t="s">
         <v>37</v>
       </c>
       <c r="E34" s="1" t="s">
-        <v>109</v>
+        <v>229</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.25">
@@ -1874,50 +1895,50 @@
         <v>111</v>
       </c>
       <c r="B35" s="3" t="s">
-        <v>107</v>
+        <v>108</v>
       </c>
       <c r="C35" s="3" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D35" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="E35" s="3" t="s">
-        <v>110</v>
+      <c r="E35" s="1" t="s">
+        <v>230</v>
       </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B36" s="3" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="C36" s="3" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="D36" s="3" t="s">
-        <v>118</v>
+        <v>37</v>
       </c>
       <c r="E36" s="1" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="B37" s="3" t="s">
-        <v>120</v>
+        <v>107</v>
       </c>
       <c r="C37" s="3" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="D37" s="3" t="s">
-        <v>118</v>
+        <v>37</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>121</v>
+        <v>110</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.25">
@@ -1925,339 +1946,339 @@
         <v>114</v>
       </c>
       <c r="B38" s="3" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="C38" s="3" t="s">
-        <v>122</v>
-      </c>
-      <c r="D38" s="1" t="s">
-        <v>163</v>
+        <v>115</v>
+      </c>
+      <c r="D38" s="3" t="s">
+        <v>118</v>
       </c>
       <c r="E38" s="1" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="B39" s="1" t="s">
-        <v>127</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>126</v>
-      </c>
-      <c r="D39" s="1" t="s">
-        <v>163</v>
-      </c>
-      <c r="E39" s="1" t="s">
-        <v>125</v>
+      <c r="B39" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="C39" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="D39" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>121</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>128</v>
-      </c>
-      <c r="B40" s="1" t="s">
-        <v>129</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>133</v>
+        <v>114</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="C40" s="3" t="s">
+        <v>122</v>
       </c>
       <c r="D40" s="1" t="s">
-        <v>36</v>
+        <v>163</v>
       </c>
       <c r="E40" s="1" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="B41" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="D41" s="1" t="s">
+        <v>163</v>
+      </c>
+      <c r="E41" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A42" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="B41" s="1" t="s">
-        <v>130</v>
-      </c>
-      <c r="C41" s="1" t="s">
-        <v>134</v>
-      </c>
-      <c r="D41" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E41" s="1" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="3" t="s">
-        <v>135</v>
-      </c>
       <c r="B42" s="1" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="D42" s="1" t="s">
         <v>36</v>
       </c>
       <c r="E42" s="1" t="s">
-        <v>225</v>
+        <v>131</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="3" t="s">
-        <v>135</v>
+      <c r="A43" s="1" t="s">
+        <v>128</v>
       </c>
       <c r="B43" s="1" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>139</v>
+        <v>134</v>
       </c>
       <c r="D43" s="1" t="s">
         <v>36</v>
       </c>
       <c r="E43" s="1" t="s">
-        <v>226</v>
+        <v>132</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="B44" s="1" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C44" s="1" t="s">
-        <v>142</v>
+        <v>138</v>
       </c>
       <c r="D44" s="1" t="s">
         <v>36</v>
       </c>
       <c r="E44" s="1" t="s">
-        <v>227</v>
+        <v>225</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="B45" s="1" t="s">
-        <v>141</v>
+        <v>137</v>
       </c>
       <c r="C45" s="1" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="D45" s="1" t="s">
         <v>36</v>
       </c>
       <c r="E45" s="1" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A46" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="D46" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E46" s="1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A47" s="3" t="s">
+        <v>144</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="C47" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D47" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E47" s="1" t="s">
         <v>228</v>
-      </c>
-    </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>148</v>
-      </c>
-      <c r="D46" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="E46" s="1" t="s">
-        <v>150</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>146</v>
-      </c>
-      <c r="C47" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="D47" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="E47" s="1" t="s">
-        <v>151</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B48" s="1" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="D48" s="1" t="s">
-        <v>118</v>
+        <v>149</v>
       </c>
       <c r="E48" s="1" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B49" s="1" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="C49" s="1" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="D49" s="1" t="s">
-        <v>118</v>
+        <v>149</v>
       </c>
       <c r="E49" s="1" t="s">
-        <v>159</v>
+        <v>151</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="B50" s="1" t="s">
-        <v>161</v>
+        <v>154</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>166</v>
+        <v>156</v>
       </c>
       <c r="D50" s="1" t="s">
         <v>118</v>
       </c>
       <c r="E50" s="1" t="s">
-        <v>164</v>
+        <v>158</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="B51" s="1" t="s">
-        <v>162</v>
+        <v>155</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>167</v>
+        <v>157</v>
       </c>
       <c r="D51" s="1" t="s">
         <v>118</v>
       </c>
       <c r="E51" s="1" t="s">
-        <v>165</v>
+        <v>159</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="B52" s="1" t="s">
-        <v>169</v>
+        <v>161</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>173</v>
+        <v>166</v>
       </c>
       <c r="D52" s="1" t="s">
-        <v>163</v>
+        <v>118</v>
       </c>
       <c r="E52" s="1" t="s">
-        <v>171</v>
+        <v>164</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>168</v>
+        <v>160</v>
       </c>
       <c r="B53" s="1" t="s">
-        <v>170</v>
+        <v>162</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>174</v>
+        <v>167</v>
       </c>
       <c r="D53" s="1" t="s">
-        <v>163</v>
+        <v>118</v>
       </c>
       <c r="E53" s="1" t="s">
-        <v>172</v>
+        <v>165</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="B54" s="1" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>180</v>
+        <v>173</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>118</v>
+        <v>163</v>
       </c>
       <c r="E54" s="1" t="s">
-        <v>178</v>
+        <v>171</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>175</v>
+        <v>168</v>
       </c>
       <c r="B55" s="1" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="D55" s="1" t="s">
-        <v>118</v>
+        <v>163</v>
       </c>
       <c r="E55" s="1" t="s">
-        <v>179</v>
+        <v>172</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="B56" s="5" t="s">
-        <v>182</v>
-      </c>
-      <c r="C56" s="5" t="s">
-        <v>196</v>
+        <v>175</v>
+      </c>
+      <c r="B56" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>180</v>
       </c>
       <c r="D56" s="1" t="s">
-        <v>163</v>
+        <v>118</v>
       </c>
       <c r="E56" s="1" t="s">
-        <v>211</v>
+        <v>178</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>210</v>
-      </c>
-      <c r="B57" s="5" t="s">
-        <v>183</v>
-      </c>
-      <c r="C57" s="5" t="s">
-        <v>197</v>
+        <v>175</v>
+      </c>
+      <c r="B57" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>181</v>
       </c>
       <c r="D57" s="1" t="s">
-        <v>163</v>
+        <v>118</v>
       </c>
       <c r="E57" s="1" t="s">
-        <v>213</v>
+        <v>179</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.25">
@@ -2265,16 +2286,16 @@
         <v>210</v>
       </c>
       <c r="B58" s="5" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
       <c r="C58" s="5" t="s">
-        <v>198</v>
+        <v>196</v>
       </c>
       <c r="D58" s="1" t="s">
         <v>163</v>
       </c>
       <c r="E58" s="1" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.25">
@@ -2282,16 +2303,16 @@
         <v>210</v>
       </c>
       <c r="B59" s="5" t="s">
-        <v>185</v>
+        <v>183</v>
       </c>
       <c r="C59" s="5" t="s">
-        <v>199</v>
+        <v>197</v>
       </c>
       <c r="D59" s="1" t="s">
         <v>163</v>
       </c>
       <c r="E59" s="1" t="s">
-        <v>212</v>
+        <v>213</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.25">
@@ -2299,16 +2320,16 @@
         <v>210</v>
       </c>
       <c r="B60" s="5" t="s">
-        <v>186</v>
+        <v>184</v>
       </c>
       <c r="C60" s="5" t="s">
-        <v>200</v>
+        <v>198</v>
       </c>
       <c r="D60" s="1" t="s">
         <v>163</v>
       </c>
       <c r="E60" s="1" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.25">
@@ -2316,16 +2337,16 @@
         <v>210</v>
       </c>
       <c r="B61" s="5" t="s">
-        <v>187</v>
+        <v>185</v>
       </c>
       <c r="C61" s="5" t="s">
-        <v>201</v>
+        <v>199</v>
       </c>
       <c r="D61" s="1" t="s">
         <v>163</v>
       </c>
       <c r="E61" s="1" t="s">
-        <v>216</v>
+        <v>212</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.25">
@@ -2333,16 +2354,16 @@
         <v>210</v>
       </c>
       <c r="B62" s="5" t="s">
-        <v>188</v>
+        <v>186</v>
       </c>
       <c r="C62" s="5" t="s">
-        <v>202</v>
+        <v>200</v>
       </c>
       <c r="D62" s="1" t="s">
         <v>163</v>
       </c>
       <c r="E62" s="1" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.25">
@@ -2350,16 +2371,16 @@
         <v>210</v>
       </c>
       <c r="B63" s="5" t="s">
-        <v>189</v>
+        <v>187</v>
       </c>
       <c r="C63" s="5" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="D63" s="1" t="s">
         <v>163</v>
       </c>
       <c r="E63" s="1" t="s">
-        <v>219</v>
+        <v>216</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.25">
@@ -2367,16 +2388,16 @@
         <v>210</v>
       </c>
       <c r="B64" s="5" t="s">
-        <v>190</v>
+        <v>188</v>
       </c>
       <c r="C64" s="5" t="s">
-        <v>204</v>
+        <v>202</v>
       </c>
       <c r="D64" s="1" t="s">
         <v>163</v>
       </c>
       <c r="E64" s="1" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
     </row>
     <row r="65" spans="1:5" x14ac:dyDescent="0.25">
@@ -2384,16 +2405,16 @@
         <v>210</v>
       </c>
       <c r="B65" s="5" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C65" s="5" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="D65" s="1" t="s">
         <v>163</v>
       </c>
       <c r="E65" s="1" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
     </row>
     <row r="66" spans="1:5" x14ac:dyDescent="0.25">
@@ -2401,16 +2422,16 @@
         <v>210</v>
       </c>
       <c r="B66" s="5" t="s">
-        <v>192</v>
+        <v>190</v>
       </c>
       <c r="C66" s="5" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="D66" s="1" t="s">
         <v>163</v>
       </c>
       <c r="E66" s="1" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.25">
@@ -2418,16 +2439,16 @@
         <v>210</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C67" s="5" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="D67" s="1" t="s">
         <v>163</v>
       </c>
       <c r="E67" s="1" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
     </row>
     <row r="68" spans="1:5" x14ac:dyDescent="0.25">
@@ -2435,16 +2456,16 @@
         <v>210</v>
       </c>
       <c r="B68" s="5" t="s">
-        <v>194</v>
+        <v>192</v>
       </c>
       <c r="C68" s="5" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="D68" s="1" t="s">
         <v>163</v>
       </c>
       <c r="E68" s="1" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
     </row>
     <row r="69" spans="1:5" x14ac:dyDescent="0.25">
@@ -2452,84 +2473,84 @@
         <v>210</v>
       </c>
       <c r="B69" s="5" t="s">
-        <v>195</v>
+        <v>193</v>
       </c>
       <c r="C69" s="5" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="D69" s="1" t="s">
         <v>163</v>
       </c>
       <c r="E69" s="1" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
     </row>
     <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>235</v>
+        <v>210</v>
       </c>
       <c r="B70" s="5" t="s">
-        <v>236</v>
+        <v>194</v>
       </c>
       <c r="C70" s="5" t="s">
-        <v>231</v>
+        <v>208</v>
       </c>
       <c r="D70" s="1" t="s">
-        <v>36</v>
+        <v>163</v>
       </c>
       <c r="E70" s="1" t="s">
-        <v>233</v>
+        <v>222</v>
       </c>
     </row>
     <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>235</v>
+        <v>210</v>
       </c>
       <c r="B71" s="5" t="s">
-        <v>237</v>
+        <v>195</v>
       </c>
       <c r="C71" s="5" t="s">
-        <v>232</v>
+        <v>209</v>
       </c>
       <c r="D71" s="1" t="s">
-        <v>36</v>
+        <v>163</v>
       </c>
       <c r="E71" s="1" t="s">
-        <v>234</v>
+        <v>224</v>
       </c>
     </row>
     <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>246</v>
+        <v>235</v>
       </c>
       <c r="B72" s="5" t="s">
-        <v>244</v>
-      </c>
-      <c r="C72" s="1" t="s">
-        <v>242</v>
+        <v>236</v>
+      </c>
+      <c r="C72" s="5" t="s">
+        <v>231</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>163</v>
+        <v>36</v>
       </c>
       <c r="E72" s="1" t="s">
-        <v>248</v>
+        <v>233</v>
       </c>
     </row>
     <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>246</v>
+        <v>235</v>
       </c>
       <c r="B73" s="5" t="s">
-        <v>245</v>
-      </c>
-      <c r="C73" s="1" t="s">
-        <v>243</v>
+        <v>237</v>
+      </c>
+      <c r="C73" s="5" t="s">
+        <v>232</v>
       </c>
       <c r="D73" s="1" t="s">
-        <v>163</v>
+        <v>36</v>
       </c>
       <c r="E73" s="1" t="s">
-        <v>247</v>
+        <v>234</v>
       </c>
     </row>
     <row r="74" spans="1:5" x14ac:dyDescent="0.25">
@@ -2537,16 +2558,16 @@
         <v>246</v>
       </c>
       <c r="B74" s="5" t="s">
-        <v>239</v>
+        <v>244</v>
       </c>
       <c r="C74" s="1" t="s">
-        <v>238</v>
+        <v>242</v>
       </c>
       <c r="D74" s="1" t="s">
         <v>163</v>
       </c>
       <c r="E74" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
@@ -2554,118 +2575,118 @@
         <v>246</v>
       </c>
       <c r="B75" s="5" t="s">
-        <v>241</v>
+        <v>245</v>
       </c>
       <c r="C75" s="1" t="s">
-        <v>240</v>
+        <v>243</v>
       </c>
       <c r="D75" s="1" t="s">
         <v>163</v>
       </c>
       <c r="E75" s="1" t="s">
-        <v>250</v>
+        <v>247</v>
       </c>
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="B76" s="1" t="s">
-        <v>252</v>
+        <v>246</v>
+      </c>
+      <c r="B76" s="5" t="s">
+        <v>239</v>
       </c>
       <c r="C76" s="1" t="s">
-        <v>256</v>
+        <v>238</v>
       </c>
       <c r="D76" s="1" t="s">
-        <v>36</v>
+        <v>163</v>
       </c>
       <c r="E76" s="1" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="B77" s="1" t="s">
-        <v>253</v>
+        <v>246</v>
+      </c>
+      <c r="B77" s="5" t="s">
+        <v>241</v>
       </c>
       <c r="C77" s="1" t="s">
-        <v>257</v>
+        <v>240</v>
       </c>
       <c r="D77" s="1" t="s">
-        <v>36</v>
+        <v>163</v>
       </c>
       <c r="E77" s="1" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>264</v>
+        <v>251</v>
       </c>
       <c r="B78" s="1" t="s">
-        <v>259</v>
+        <v>252</v>
       </c>
       <c r="C78" s="1" t="s">
-        <v>258</v>
+        <v>256</v>
       </c>
       <c r="D78" s="1" t="s">
         <v>36</v>
       </c>
       <c r="E78" s="1" t="s">
-        <v>261</v>
+        <v>254</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>264</v>
+        <v>251</v>
       </c>
       <c r="B79" s="1" t="s">
-        <v>260</v>
+        <v>253</v>
       </c>
       <c r="C79" s="1" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="D79" s="1" t="s">
         <v>36</v>
       </c>
       <c r="E79" s="1" t="s">
-        <v>262</v>
+        <v>255</v>
       </c>
     </row>
     <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="B80" s="6" t="s">
-        <v>266</v>
-      </c>
-      <c r="C80" s="6" t="s">
-        <v>270</v>
-      </c>
-      <c r="D80" s="6" t="s">
-        <v>118</v>
+        <v>264</v>
+      </c>
+      <c r="B80" s="1" t="s">
+        <v>259</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>258</v>
+      </c>
+      <c r="D80" s="1" t="s">
+        <v>36</v>
       </c>
       <c r="E80" s="1" t="s">
-        <v>274</v>
+        <v>261</v>
       </c>
     </row>
     <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>265</v>
-      </c>
-      <c r="B81" s="6" t="s">
-        <v>267</v>
-      </c>
-      <c r="C81" s="6" t="s">
-        <v>271</v>
-      </c>
-      <c r="D81" s="6" t="s">
-        <v>118</v>
+        <v>264</v>
+      </c>
+      <c r="B81" s="1" t="s">
+        <v>260</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="D81" s="1" t="s">
+        <v>36</v>
       </c>
       <c r="E81" s="1" t="s">
-        <v>276</v>
+        <v>262</v>
       </c>
     </row>
     <row r="82" spans="1:5" x14ac:dyDescent="0.25">
@@ -2673,16 +2694,16 @@
         <v>265</v>
       </c>
       <c r="B82" s="6" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C82" s="6" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="D82" s="6" t="s">
         <v>118</v>
       </c>
       <c r="E82" s="1" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="83" spans="1:5" x14ac:dyDescent="0.25">
@@ -2690,49 +2711,83 @@
         <v>265</v>
       </c>
       <c r="B83" s="6" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C83" s="6" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="D83" s="6" t="s">
         <v>118</v>
       </c>
       <c r="E83" s="1" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>278</v>
+        <v>265</v>
       </c>
       <c r="B84" s="6" t="s">
-        <v>279</v>
+        <v>268</v>
       </c>
       <c r="C84" s="6" t="s">
-        <v>281</v>
-      </c>
-      <c r="D84" s="1" t="s">
-        <v>36</v>
+        <v>272</v>
+      </c>
+      <c r="D84" s="6" t="s">
+        <v>118</v>
       </c>
       <c r="E84" s="1" t="s">
-        <v>282</v>
+        <v>275</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
+        <v>265</v>
+      </c>
+      <c r="B85" s="6" t="s">
+        <v>269</v>
+      </c>
+      <c r="C85" s="6" t="s">
+        <v>273</v>
+      </c>
+      <c r="D85" s="6" t="s">
+        <v>118</v>
+      </c>
+      <c r="E85" s="1" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A86" s="1" t="s">
         <v>278</v>
       </c>
-      <c r="B85" s="6" t="s">
+      <c r="B86" s="6" t="s">
+        <v>279</v>
+      </c>
+      <c r="C86" s="6" t="s">
+        <v>281</v>
+      </c>
+      <c r="D86" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E86" s="1" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A87" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="B87" s="6" t="s">
         <v>280</v>
       </c>
-      <c r="C85" s="6" t="s">
+      <c r="C87" s="6" t="s">
         <v>283</v>
       </c>
-      <c r="D85" s="1" t="s">
+      <c r="D87" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="E85" s="1" t="s">
+      <c r="E87" s="1" t="s">
         <v>284</v>
       </c>
     </row>

</xml_diff>

<commit_message>
0.9 - pandas 2.1 refactorng, principal switch icon
</commit_message>
<xml_diff>
--- a/dtln_device_location.xlsx
+++ b/dtln_device_location.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20403"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20404"/>
   <workbookPr codeName="ЭтаКнига" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kavlasenko\Documents\05.PYTHON\Projects\san_report_automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65B7EBBF-EA94-40B1-8682-9E75F2FBF222}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{720849E7-5DF2-4735-AD05-3FF77BE4A891}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="34335" windowHeight="11730" xr2:uid="{224B2F82-8F05-438B-BF5A-3CD3FE39A21B}"/>
   </bookViews>
@@ -1018,12 +1018,6 @@
     <t>5H3E110 un39</t>
   </si>
   <si>
-    <t xml:space="preserve">H4B010 un41	</t>
-  </si>
-  <si>
-    <t xml:space="preserve">H4B020 un41	</t>
-  </si>
-  <si>
     <t>10:00:d8:1f:cc:8a:56:b0</t>
   </si>
   <si>
@@ -1070,6 +1064,12 @@
   </si>
   <si>
     <t>10:00:00:27:f8:0b:fe:79</t>
+  </si>
+  <si>
+    <t>H4B020 un41</t>
+  </si>
+  <si>
+    <t>H4B010 un41</t>
   </si>
 </sst>
 </file>
@@ -1468,8 +1468,8 @@
   <sheetPr codeName="Лист1"/>
   <dimension ref="A1:E105"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="B100" sqref="B100"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="F94" sqref="F94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3002,7 +3002,7 @@
         <v>324</v>
       </c>
       <c r="C90" s="6" t="s">
-        <v>331</v>
+        <v>329</v>
       </c>
       <c r="D90" s="1" t="s">
         <v>36</v>
@@ -3019,13 +3019,13 @@
         <v>325</v>
       </c>
       <c r="C91" s="6" t="s">
-        <v>332</v>
+        <v>330</v>
       </c>
       <c r="D91" s="1" t="s">
         <v>36</v>
       </c>
       <c r="E91" s="1" t="s">
-        <v>333</v>
+        <v>331</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.25">
@@ -3042,7 +3042,7 @@
         <v>36</v>
       </c>
       <c r="E92" s="1" t="s">
-        <v>329</v>
+        <v>346</v>
       </c>
     </row>
     <row r="93" spans="1:5" x14ac:dyDescent="0.25">
@@ -3059,7 +3059,7 @@
         <v>36</v>
       </c>
       <c r="E93" s="1" t="s">
-        <v>330</v>
+        <v>345</v>
       </c>
     </row>
     <row r="94" spans="1:5" x14ac:dyDescent="0.25">
@@ -3200,70 +3200,70 @@
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="D102" s="1" t="s">
         <v>160</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
+        <v>340</v>
+      </c>
+      <c r="B103" s="1" t="s">
+        <v>333</v>
+      </c>
+      <c r="C103" s="1" t="s">
         <v>342</v>
-      </c>
-      <c r="B103" s="1" t="s">
-        <v>335</v>
-      </c>
-      <c r="C103" s="1" t="s">
-        <v>344</v>
       </c>
       <c r="D103" s="1" t="s">
         <v>160</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>336</v>
+        <v>334</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>345</v>
+        <v>343</v>
       </c>
       <c r="D104" s="1" t="s">
         <v>160</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>340</v>
+        <v>338</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>337</v>
+        <v>335</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>346</v>
+        <v>344</v>
       </c>
       <c r="D105" s="1" t="s">
         <v>160</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>341</v>
+        <v>339</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
0.91 - visio switch entry and middle shapes
</commit_message>
<xml_diff>
--- a/dtln_device_location.xlsx
+++ b/dtln_device_location.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kavlasenko\Documents\05.PYTHON\Projects\san_report_automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{720849E7-5DF2-4735-AD05-3FF77BE4A891}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BDC7A89-1050-4474-BBCF-482FB3D11C55}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="34335" windowHeight="11730" xr2:uid="{224B2F82-8F05-438B-BF5A-3CD3FE39A21B}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="553" uniqueCount="347">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="354">
   <si>
     <t>san01-nord</t>
   </si>
@@ -1070,6 +1070,27 @@
   </si>
   <si>
     <t>H4B010 un41</t>
+  </si>
+  <si>
+    <t>10:00:c4:f5:7c:9e:0f:a0</t>
+  </si>
+  <si>
+    <t>Nsk</t>
+  </si>
+  <si>
+    <t>san15-nsk</t>
+  </si>
+  <si>
+    <t>san16-nsk</t>
+  </si>
+  <si>
+    <t>2_4_17 un36</t>
+  </si>
+  <si>
+    <t>2_4_16 un36</t>
+  </si>
+  <si>
+    <t>10:00:c4:f5:7c:a4:bc:20</t>
   </si>
 </sst>
 </file>
@@ -1466,10 +1487,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FE7DAD2-DE8B-4AD9-A367-2ED64EC8ED26}">
   <sheetPr codeName="Лист1"/>
-  <dimension ref="A1:E105"/>
+  <dimension ref="A1:E107"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
-      <selection activeCell="F94" sqref="F94"/>
+    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
+      <selection activeCell="C113" sqref="C113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3264,6 +3285,40 @@
       </c>
       <c r="E105" s="1" t="s">
         <v>339</v>
+      </c>
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A106" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="B106" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="C106" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="D106" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="E106" s="1" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A107" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="B107" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="D107" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="E107" s="1" t="s">
+        <v>352</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
v0.94 - Clock server changed counter is added to the ralog analysis
</commit_message>
<xml_diff>
--- a/dtln_device_location.xlsx
+++ b/dtln_device_location.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kavlasenko\Documents\05.PYTHON\Projects\san_report_automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4BDC7A89-1050-4474-BBCF-482FB3D11C55}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ED9CB07B-F2BF-4608-8B81-6F06598C2E97}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="34335" windowHeight="11730" xr2:uid="{224B2F82-8F05-438B-BF5A-3CD3FE39A21B}"/>
   </bookViews>
@@ -17,7 +17,7 @@
     <sheet name="Лист1" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">switch_rack!$A$1:$E$101</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">switch_rack!$A$1:$E$103</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="563" uniqueCount="354">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="368">
   <si>
     <t>san01-nord</t>
   </si>
@@ -1091,6 +1091,48 @@
   </si>
   <si>
     <t>10:00:c4:f5:7c:a4:bc:20</t>
+  </si>
+  <si>
+    <t>o3-g630-003-vc01-f1</t>
+  </si>
+  <si>
+    <t>o3-g630-004-vc01-f2</t>
+  </si>
+  <si>
+    <t>Brocade G630</t>
+  </si>
+  <si>
+    <t>1H15C140 un40-41</t>
+  </si>
+  <si>
+    <t>1H15C180 un40-41</t>
+  </si>
+  <si>
+    <t>10:00:88:94:71:bd:43:20</t>
+  </si>
+  <si>
+    <t>10:00:88:94:71:c2:fe:40</t>
+  </si>
+  <si>
+    <t>VC02</t>
+  </si>
+  <si>
+    <t>n4-g620-003-vc02-f1</t>
+  </si>
+  <si>
+    <t>n4-g620-004-vc02-f2</t>
+  </si>
+  <si>
+    <t>10:00:88:94:71:45:03:00</t>
+  </si>
+  <si>
+    <t>10:00:d8:1f:cc:a1:cb:80</t>
+  </si>
+  <si>
+    <t>6H6H150 un38</t>
+  </si>
+  <si>
+    <t>6H6H170 un38</t>
   </si>
 </sst>
 </file>
@@ -1176,7 +1218,18 @@
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -1487,10 +1540,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5FE7DAD2-DE8B-4AD9-A367-2ED64EC8ED26}">
   <sheetPr codeName="Лист1"/>
-  <dimension ref="A1:E107"/>
+  <dimension ref="A1:E111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A80" workbookViewId="0">
-      <selection activeCell="C113" sqref="C113"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="G117" sqref="G117"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3119,36 +3172,36 @@
     </row>
     <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>315</v>
-      </c>
-      <c r="B96" s="1" t="s">
-        <v>303</v>
-      </c>
-      <c r="C96" s="1" t="s">
-        <v>304</v>
+        <v>273</v>
+      </c>
+      <c r="B96" s="6" t="s">
+        <v>354</v>
+      </c>
+      <c r="C96" s="6" t="s">
+        <v>359</v>
       </c>
       <c r="D96" s="1" t="s">
-        <v>160</v>
+        <v>356</v>
       </c>
       <c r="E96" s="1" t="s">
-        <v>316</v>
+        <v>357</v>
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>315</v>
-      </c>
-      <c r="B97" s="1" t="s">
-        <v>305</v>
-      </c>
-      <c r="C97" s="1" t="s">
-        <v>306</v>
+        <v>273</v>
+      </c>
+      <c r="B97" s="6" t="s">
+        <v>355</v>
+      </c>
+      <c r="C97" s="6" t="s">
+        <v>360</v>
       </c>
       <c r="D97" s="1" t="s">
-        <v>160</v>
+        <v>356</v>
       </c>
       <c r="E97" s="1" t="s">
-        <v>318</v>
+        <v>358</v>
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.25">
@@ -3156,16 +3209,16 @@
         <v>315</v>
       </c>
       <c r="B98" s="1" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="D98" s="1" t="s">
         <v>160</v>
       </c>
       <c r="E98" s="1" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.25">
@@ -3173,16 +3226,16 @@
         <v>315</v>
       </c>
       <c r="B99" s="1" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>310</v>
+        <v>306</v>
       </c>
       <c r="D99" s="1" t="s">
         <v>160</v>
       </c>
       <c r="E99" s="1" t="s">
-        <v>317</v>
+        <v>318</v>
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.25">
@@ -3190,16 +3243,16 @@
         <v>315</v>
       </c>
       <c r="B100" s="1" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>312</v>
+        <v>308</v>
       </c>
       <c r="D100" s="1" t="s">
         <v>160</v>
       </c>
       <c r="E100" s="1" t="s">
-        <v>319</v>
+        <v>320</v>
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.25">
@@ -3207,50 +3260,50 @@
         <v>315</v>
       </c>
       <c r="B101" s="1" t="s">
-        <v>313</v>
+        <v>309</v>
       </c>
       <c r="C101" s="1" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="D101" s="1" t="s">
         <v>160</v>
       </c>
       <c r="E101" s="1" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
-        <v>340</v>
+        <v>315</v>
       </c>
       <c r="B102" s="1" t="s">
-        <v>332</v>
+        <v>311</v>
       </c>
       <c r="C102" s="1" t="s">
-        <v>341</v>
+        <v>312</v>
       </c>
       <c r="D102" s="1" t="s">
         <v>160</v>
       </c>
       <c r="E102" s="1" t="s">
-        <v>336</v>
+        <v>319</v>
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>340</v>
+        <v>315</v>
       </c>
       <c r="B103" s="1" t="s">
-        <v>333</v>
+        <v>313</v>
       </c>
       <c r="C103" s="1" t="s">
-        <v>342</v>
+        <v>314</v>
       </c>
       <c r="D103" s="1" t="s">
         <v>160</v>
       </c>
       <c r="E103" s="1" t="s">
-        <v>337</v>
+        <v>321</v>
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.25">
@@ -3258,16 +3311,16 @@
         <v>340</v>
       </c>
       <c r="B104" s="1" t="s">
-        <v>334</v>
+        <v>332</v>
       </c>
       <c r="C104" s="1" t="s">
-        <v>343</v>
+        <v>341</v>
       </c>
       <c r="D104" s="1" t="s">
         <v>160</v>
       </c>
       <c r="E104" s="1" t="s">
-        <v>338</v>
+        <v>336</v>
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.25">
@@ -3275,53 +3328,124 @@
         <v>340</v>
       </c>
       <c r="B105" s="1" t="s">
-        <v>335</v>
+        <v>333</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>344</v>
+        <v>342</v>
       </c>
       <c r="D105" s="1" t="s">
         <v>160</v>
       </c>
       <c r="E105" s="1" t="s">
-        <v>339</v>
+        <v>337</v>
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>348</v>
+        <v>340</v>
       </c>
       <c r="B106" s="1" t="s">
-        <v>349</v>
+        <v>334</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="D106" s="1" t="s">
         <v>160</v>
       </c>
       <c r="E106" s="1" t="s">
-        <v>351</v>
+        <v>338</v>
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>348</v>
+        <v>340</v>
       </c>
       <c r="B107" s="1" t="s">
-        <v>350</v>
+        <v>335</v>
       </c>
       <c r="C107" s="1" t="s">
-        <v>353</v>
+        <v>344</v>
       </c>
       <c r="D107" s="1" t="s">
         <v>160</v>
       </c>
       <c r="E107" s="1" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A108" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="B108" s="1" t="s">
+        <v>349</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>347</v>
+      </c>
+      <c r="D108" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="E108" s="1" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A109" s="1" t="s">
+        <v>348</v>
+      </c>
+      <c r="B109" s="1" t="s">
+        <v>350</v>
+      </c>
+      <c r="C109" s="1" t="s">
+        <v>353</v>
+      </c>
+      <c r="D109" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="E109" s="1" t="s">
         <v>352</v>
       </c>
     </row>
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A110" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="B110" s="1" t="s">
+        <v>362</v>
+      </c>
+      <c r="C110" s="1" t="s">
+        <v>364</v>
+      </c>
+      <c r="D110" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E110" s="1" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A111" s="1" t="s">
+        <v>361</v>
+      </c>
+      <c r="B111" s="1" t="s">
+        <v>363</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>365</v>
+      </c>
+      <c r="D111" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="E111" s="1" t="s">
+        <v>367</v>
+      </c>
+    </row>
   </sheetData>
+  <conditionalFormatting sqref="C1:C1048576">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>

</xml_diff>